<commit_message>
All working without Sources
</commit_message>
<xml_diff>
--- a/Testing/CPS/CPS_CAS 102-76-1.xlsx
+++ b/Testing/CPS/CPS_CAS 102-76-1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sara.lentink/Arche Dropbox/C2C/08_Chemical Profiling/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/arche/Documents/Python/C2Cautomatisation/Testing/CPS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14AFD4A6-C89F-FF4C-AF0F-FC5CC6E12EBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE764C97-F0E4-B74C-9FFF-6EC3B56963B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17320" yWindow="-22160" windowWidth="27660" windowHeight="17340" xr2:uid="{4DA62B78-EFF6-274F-9A3C-3E5FD52E9962}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{4DA62B78-EFF6-274F-9A3C-3E5FD52E9962}"/>
   </bookViews>
   <sheets>
     <sheet name="102-76-1" sheetId="1" r:id="rId1"/>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="131">
   <si>
     <t>Arche</t>
   </si>
@@ -445,6 +445,9 @@
   </si>
   <si>
     <t>Not sensitzing according to testing</t>
+  </si>
+  <si>
+    <t>Carc. 1B: H350: May cause cancer</t>
   </si>
 </sst>
 </file>
@@ -1066,6 +1069,80 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1096,83 +1173,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3909,8 +3912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B588471F-4DE3-3B49-B52D-46DD988FA694}">
   <dimension ref="A1:L155"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="M118" sqref="M118"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3991,17 +3994,17 @@
       <c r="B6" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="D6" s="119"/>
-      <c r="E6" s="119"/>
-      <c r="F6" s="119" t="s">
+      <c r="D6" s="85"/>
+      <c r="E6" s="85"/>
+      <c r="F6" s="85" t="s">
         <v>114</v>
       </c>
-      <c r="G6" s="119"/>
-      <c r="H6" s="119" t="s">
+      <c r="G6" s="85"/>
+      <c r="H6" s="85" t="s">
         <v>115</v>
       </c>
-      <c r="I6" s="119"/>
-      <c r="J6" s="120">
+      <c r="I6" s="85"/>
+      <c r="J6" s="86">
         <v>41838</v>
       </c>
       <c r="K6" s="8" t="s">
@@ -4010,50 +4013,50 @@
       <c r="L6" s="3"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="119" t="s">
+      <c r="B7" s="85" t="s">
         <v>116</v>
       </c>
-      <c r="D7" s="119"/>
-      <c r="E7" s="119"/>
-      <c r="F7" s="119"/>
-      <c r="G7" s="119"/>
-      <c r="H7" s="119" t="s">
+      <c r="D7" s="85"/>
+      <c r="E7" s="85"/>
+      <c r="F7" s="85"/>
+      <c r="G7" s="85"/>
+      <c r="H7" s="85" t="s">
         <v>117</v>
       </c>
-      <c r="I7" s="119"/>
-      <c r="J7" s="121">
+      <c r="I7" s="85"/>
+      <c r="J7" s="87">
         <v>44852</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="119" t="s">
+      <c r="B8" s="85" t="s">
         <v>118</v>
       </c>
-      <c r="C8" s="119"/>
-      <c r="D8" s="119"/>
-      <c r="E8" s="119"/>
-      <c r="F8" s="119"/>
-      <c r="G8" s="119"/>
-      <c r="H8" s="119" t="s">
+      <c r="C8" s="85"/>
+      <c r="D8" s="85"/>
+      <c r="E8" s="85"/>
+      <c r="F8" s="85"/>
+      <c r="G8" s="85"/>
+      <c r="H8" s="85" t="s">
         <v>119</v>
       </c>
-      <c r="I8" s="119"/>
-      <c r="J8" s="121">
+      <c r="I8" s="85"/>
+      <c r="J8" s="87">
         <v>45855</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="119" t="s">
+      <c r="B9" s="85" t="s">
         <v>120</v>
       </c>
-      <c r="C9" s="119"/>
-      <c r="D9" s="119"/>
-      <c r="E9" s="119"/>
-      <c r="F9" s="119"/>
-      <c r="G9" s="119"/>
-      <c r="H9" s="119"/>
-      <c r="I9" s="119"/>
-      <c r="J9" s="119"/>
+      <c r="C9" s="85"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="C10" s="11"/>
@@ -4099,18 +4102,18 @@
       <c r="A16" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="115" t="s">
+      <c r="B16" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="116"/>
-      <c r="D16" s="116"/>
-      <c r="E16" s="116"/>
-      <c r="F16" s="116"/>
-      <c r="G16" s="117"/>
-      <c r="H16" s="107" t="s">
+      <c r="C16" s="90"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="91"/>
+      <c r="H16" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="I16" s="108"/>
+      <c r="I16" s="93"/>
       <c r="J16" s="18" t="s">
         <v>16</v>
       </c>
@@ -4144,25 +4147,25 @@
       <c r="B18" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C18" s="95" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18" s="110"/>
-      <c r="E18" s="110"/>
+      <c r="C18" s="94" t="s">
+        <v>130</v>
+      </c>
+      <c r="D18" s="95"/>
+      <c r="E18" s="95"/>
       <c r="F18" s="96"/>
       <c r="H18" s="26"/>
       <c r="I18" s="27"/>
       <c r="J18" s="25"/>
-      <c r="K18" s="118"/>
-      <c r="L18" s="98"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="88"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="28"/>
       <c r="H19" s="29"/>
       <c r="I19" s="30"/>
       <c r="J19" s="28"/>
-      <c r="K19" s="100"/>
-      <c r="L19" s="98"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="88"/>
     </row>
     <row r="20" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="31"/>
@@ -4185,16 +4188,16 @@
       <c r="H21" s="29"/>
       <c r="I21" s="30"/>
       <c r="J21" s="28"/>
-      <c r="K21" s="100"/>
-      <c r="L21" s="98"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="88"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="28"/>
       <c r="H22" s="29"/>
       <c r="I22" s="30"/>
       <c r="J22" s="28"/>
-      <c r="K22" s="100"/>
-      <c r="L22" s="98"/>
+      <c r="K22" s="98"/>
+      <c r="L22" s="88"/>
     </row>
     <row r="23" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="36"/>
@@ -4217,17 +4220,17 @@
       <c r="B24" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="95" t="s">
+      <c r="C24" s="94" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="110"/>
-      <c r="E24" s="110"/>
+      <c r="D24" s="95"/>
+      <c r="E24" s="95"/>
       <c r="F24" s="96"/>
       <c r="H24" s="29"/>
       <c r="I24" s="30"/>
       <c r="J24" s="28"/>
-      <c r="K24" s="113"/>
-      <c r="L24" s="98"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="88"/>
     </row>
     <row r="25" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="40" t="s">
@@ -4236,10 +4239,10 @@
       <c r="B25" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C25" s="95" t="s">
+      <c r="C25" s="94" t="s">
         <v>121</v>
       </c>
-      <c r="D25" s="110"/>
+      <c r="D25" s="95"/>
       <c r="E25" s="96"/>
       <c r="F25" s="41" t="s">
         <v>122</v>
@@ -4249,18 +4252,18 @@
       </c>
       <c r="I25" s="30"/>
       <c r="J25" s="28"/>
-      <c r="K25" s="114"/>
-      <c r="L25" s="98"/>
+      <c r="K25" s="100"/>
+      <c r="L25" s="88"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="28"/>
       <c r="B26" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C26" s="95" t="s">
+      <c r="C26" s="94" t="s">
         <v>124</v>
       </c>
-      <c r="D26" s="110"/>
+      <c r="D26" s="95"/>
       <c r="E26" s="96"/>
       <c r="F26" s="41" t="s">
         <v>122</v>
@@ -4268,16 +4271,16 @@
       <c r="H26" s="29"/>
       <c r="I26" s="30"/>
       <c r="J26" s="28"/>
-      <c r="K26" s="114"/>
-      <c r="L26" s="98"/>
+      <c r="K26" s="100"/>
+      <c r="L26" s="88"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="30"/>
       <c r="H27" s="29"/>
       <c r="I27" s="30"/>
       <c r="J27" s="28"/>
-      <c r="K27" s="114"/>
-      <c r="L27" s="98"/>
+      <c r="K27" s="100"/>
+      <c r="L27" s="88"/>
     </row>
     <row r="28" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="31"/>
@@ -4300,15 +4303,15 @@
       <c r="B29" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="95"/>
-      <c r="D29" s="110"/>
-      <c r="E29" s="110"/>
+      <c r="C29" s="94"/>
+      <c r="D29" s="95"/>
+      <c r="E29" s="95"/>
       <c r="F29" s="96"/>
       <c r="H29" s="29"/>
       <c r="I29" s="30"/>
       <c r="J29" s="28"/>
-      <c r="K29" s="97"/>
-      <c r="L29" s="98"/>
+      <c r="K29" s="101"/>
+      <c r="L29" s="88"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="28"/>
@@ -4327,16 +4330,16 @@
       </c>
       <c r="I30" s="30"/>
       <c r="J30" s="28"/>
-      <c r="K30" s="97"/>
-      <c r="L30" s="98"/>
+      <c r="K30" s="101"/>
+      <c r="L30" s="88"/>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="28"/>
       <c r="H31" s="29"/>
       <c r="I31" s="30"/>
       <c r="J31" s="28"/>
-      <c r="K31" s="97"/>
-      <c r="L31" s="98"/>
+      <c r="K31" s="101"/>
+      <c r="L31" s="88"/>
     </row>
     <row r="32" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="36"/>
@@ -4359,15 +4362,15 @@
       <c r="B33" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="95"/>
-      <c r="D33" s="110"/>
-      <c r="E33" s="110"/>
+      <c r="C33" s="94"/>
+      <c r="D33" s="95"/>
+      <c r="E33" s="95"/>
       <c r="F33" s="96"/>
       <c r="H33" s="29"/>
       <c r="I33" s="30"/>
       <c r="J33" s="28"/>
-      <c r="K33" s="97"/>
-      <c r="L33" s="98"/>
+      <c r="K33" s="101"/>
+      <c r="L33" s="88"/>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" s="30"/>
@@ -4386,16 +4389,16 @@
       </c>
       <c r="I34" s="30"/>
       <c r="J34" s="28"/>
-      <c r="K34" s="97"/>
-      <c r="L34" s="98"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="88"/>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" s="30"/>
       <c r="H35" s="29"/>
       <c r="I35" s="30"/>
       <c r="J35" s="28"/>
-      <c r="K35" s="97"/>
-      <c r="L35" s="98"/>
+      <c r="K35" s="101"/>
+      <c r="L35" s="88"/>
     </row>
     <row r="36" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="36"/>
@@ -4418,8 +4421,8 @@
       <c r="G37" s="30"/>
       <c r="I37" s="30"/>
       <c r="J37" s="28"/>
-      <c r="K37" s="112"/>
-      <c r="L37" s="98"/>
+      <c r="K37" s="102"/>
+      <c r="L37" s="88"/>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" s="30"/>
@@ -4427,8 +4430,8 @@
       <c r="G38" s="30"/>
       <c r="I38" s="30"/>
       <c r="J38" s="28"/>
-      <c r="K38" s="112"/>
-      <c r="L38" s="98"/>
+      <c r="K38" s="102"/>
+      <c r="L38" s="88"/>
     </row>
     <row r="39" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
@@ -4451,30 +4454,30 @@
       <c r="B40" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="95"/>
-      <c r="D40" s="110"/>
-      <c r="E40" s="110"/>
+      <c r="C40" s="94"/>
+      <c r="D40" s="95"/>
+      <c r="E40" s="95"/>
       <c r="F40" s="96"/>
       <c r="G40" s="30"/>
       <c r="I40" s="30"/>
       <c r="J40" s="28"/>
-      <c r="K40" s="97"/>
-      <c r="L40" s="98"/>
+      <c r="K40" s="101"/>
+      <c r="L40" s="88"/>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A41" s="30"/>
       <c r="B41" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="95"/>
-      <c r="D41" s="110"/>
-      <c r="E41" s="110"/>
+      <c r="C41" s="94"/>
+      <c r="D41" s="95"/>
+      <c r="E41" s="95"/>
       <c r="F41" s="96"/>
       <c r="G41" s="30"/>
       <c r="I41" s="30"/>
       <c r="J41" s="28"/>
-      <c r="K41" s="97"/>
-      <c r="L41" s="98"/>
+      <c r="K41" s="101"/>
+      <c r="L41" s="88"/>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B42" s="47" t="s">
@@ -4493,8 +4496,8 @@
       </c>
       <c r="I42" s="30"/>
       <c r="J42" s="28"/>
-      <c r="K42" s="97"/>
-      <c r="L42" s="98"/>
+      <c r="K42" s="101"/>
+      <c r="L42" s="88"/>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B43" s="47" t="s">
@@ -4510,16 +4513,16 @@
       <c r="H43" s="29"/>
       <c r="I43" s="30"/>
       <c r="J43" s="28"/>
-      <c r="K43" s="97"/>
-      <c r="L43" s="98"/>
+      <c r="K43" s="101"/>
+      <c r="L43" s="88"/>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A44" s="30"/>
       <c r="G44" s="30"/>
       <c r="I44" s="30"/>
       <c r="J44" s="28"/>
-      <c r="K44" s="97"/>
-      <c r="L44" s="98"/>
+      <c r="K44" s="101"/>
+      <c r="L44" s="88"/>
     </row>
     <row r="45" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="31"/>
@@ -4542,31 +4545,31 @@
       <c r="B46" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="95"/>
-      <c r="D46" s="110"/>
-      <c r="E46" s="110"/>
+      <c r="C46" s="94"/>
+      <c r="D46" s="95"/>
+      <c r="E46" s="95"/>
       <c r="F46" s="96"/>
       <c r="G46" s="30"/>
       <c r="I46" s="30"/>
       <c r="J46" s="28"/>
-      <c r="K46" s="98"/>
-      <c r="L46" s="98"/>
+      <c r="K46" s="88"/>
+      <c r="L46" s="88"/>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A47" s="30"/>
       <c r="B47" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C47" s="95"/>
-      <c r="D47" s="110"/>
-      <c r="E47" s="110"/>
+      <c r="C47" s="94"/>
+      <c r="D47" s="95"/>
+      <c r="E47" s="95"/>
       <c r="F47" s="96"/>
       <c r="G47" s="30"/>
       <c r="H47" s="29"/>
       <c r="I47" s="30"/>
       <c r="J47" s="28"/>
-      <c r="K47" s="98"/>
-      <c r="L47" s="98"/>
+      <c r="K47" s="88"/>
+      <c r="L47" s="88"/>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A48" s="30"/>
@@ -4586,8 +4589,8 @@
       </c>
       <c r="I48" s="30"/>
       <c r="J48" s="28"/>
-      <c r="K48" s="98"/>
-      <c r="L48" s="98"/>
+      <c r="K48" s="88"/>
+      <c r="L48" s="88"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A49" s="30"/>
@@ -4602,16 +4605,16 @@
       <c r="G49" s="30"/>
       <c r="I49" s="30"/>
       <c r="J49" s="28"/>
-      <c r="K49" s="98"/>
-      <c r="L49" s="98"/>
+      <c r="K49" s="88"/>
+      <c r="L49" s="88"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A50" s="30"/>
       <c r="G50" s="30"/>
       <c r="I50" s="30"/>
       <c r="J50" s="28"/>
-      <c r="K50" s="98"/>
-      <c r="L50" s="98"/>
+      <c r="K50" s="88"/>
+      <c r="L50" s="88"/>
     </row>
     <row r="51" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="31"/>
@@ -4634,26 +4637,26 @@
       <c r="B52" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C52" s="95"/>
-      <c r="D52" s="110"/>
-      <c r="E52" s="110"/>
+      <c r="C52" s="94"/>
+      <c r="D52" s="95"/>
+      <c r="E52" s="95"/>
       <c r="F52" s="96"/>
       <c r="G52" s="30"/>
       <c r="I52" s="30"/>
       <c r="J52" s="28"/>
-      <c r="K52" s="97" t="s">
+      <c r="K52" s="101" t="s">
         <v>127</v>
       </c>
-      <c r="L52" s="98"/>
+      <c r="L52" s="88"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A53" s="30"/>
       <c r="B53" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C53" s="95"/>
-      <c r="D53" s="110"/>
-      <c r="E53" s="110"/>
+      <c r="C53" s="94"/>
+      <c r="D53" s="95"/>
+      <c r="E53" s="95"/>
       <c r="F53" s="96"/>
       <c r="G53" s="30"/>
       <c r="H53" t="s">
@@ -4661,8 +4664,8 @@
       </c>
       <c r="I53" s="30"/>
       <c r="J53" s="28"/>
-      <c r="K53" s="97"/>
-      <c r="L53" s="98"/>
+      <c r="K53" s="101"/>
+      <c r="L53" s="88"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A54" s="30"/>
@@ -4677,8 +4680,8 @@
       <c r="H54" s="29"/>
       <c r="I54" s="30"/>
       <c r="J54" s="28"/>
-      <c r="K54" s="97"/>
-      <c r="L54" s="98"/>
+      <c r="K54" s="101"/>
+      <c r="L54" s="88"/>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B55" s="47" t="s">
@@ -4691,8 +4694,8 @@
       <c r="G55" s="30"/>
       <c r="I55" s="30"/>
       <c r="J55" s="28"/>
-      <c r="K55" s="97"/>
-      <c r="L55" s="98"/>
+      <c r="K55" s="101"/>
+      <c r="L55" s="88"/>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A56" s="30"/>
@@ -4702,8 +4705,8 @@
       <c r="G56" s="30"/>
       <c r="I56" s="30"/>
       <c r="J56" s="28"/>
-      <c r="K56" s="97"/>
-      <c r="L56" s="98"/>
+      <c r="K56" s="101"/>
+      <c r="L56" s="88"/>
     </row>
     <row r="57" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="31"/>
@@ -4726,11 +4729,11 @@
       <c r="B58" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C58" s="95" t="s">
+      <c r="C58" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="D58" s="110"/>
-      <c r="E58" s="110"/>
+      <c r="D58" s="95"/>
+      <c r="E58" s="95"/>
       <c r="F58" s="96"/>
       <c r="G58" s="30"/>
       <c r="H58" t="s">
@@ -4738,40 +4741,40 @@
       </c>
       <c r="I58" s="30"/>
       <c r="J58" s="28"/>
-      <c r="K58" s="97"/>
-      <c r="L58" s="98"/>
+      <c r="K58" s="101"/>
+      <c r="L58" s="88"/>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A59" s="30"/>
       <c r="B59" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="95" t="s">
+      <c r="C59" s="94" t="s">
         <v>128</v>
       </c>
-      <c r="D59" s="110"/>
-      <c r="E59" s="110"/>
+      <c r="D59" s="95"/>
+      <c r="E59" s="95"/>
       <c r="F59" s="96"/>
       <c r="G59" s="30"/>
       <c r="I59" s="30"/>
       <c r="J59" s="28"/>
-      <c r="K59" s="97"/>
-      <c r="L59" s="98"/>
+      <c r="K59" s="101"/>
+      <c r="L59" s="88"/>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A60" s="30"/>
       <c r="B60" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C60" s="95"/>
-      <c r="D60" s="110"/>
-      <c r="E60" s="110"/>
+      <c r="C60" s="94"/>
+      <c r="D60" s="95"/>
+      <c r="E60" s="95"/>
       <c r="F60" s="96"/>
       <c r="G60" s="30"/>
       <c r="I60" s="30"/>
       <c r="J60" s="28"/>
-      <c r="K60" s="97"/>
-      <c r="L60" s="98"/>
+      <c r="K60" s="101"/>
+      <c r="L60" s="88"/>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A61" s="30"/>
@@ -4783,16 +4786,16 @@
       <c r="G61" s="30"/>
       <c r="I61" s="30"/>
       <c r="J61" s="28"/>
-      <c r="K61" s="97"/>
-      <c r="L61" s="98"/>
+      <c r="K61" s="101"/>
+      <c r="L61" s="88"/>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A62" s="30"/>
       <c r="G62" s="30"/>
       <c r="I62" s="30"/>
       <c r="J62" s="28"/>
-      <c r="K62" s="97"/>
-      <c r="L62" s="98"/>
+      <c r="K62" s="101"/>
+      <c r="L62" s="88"/>
     </row>
     <row r="63" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="31"/>
@@ -4815,11 +4818,11 @@
       <c r="B64" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C64" s="95" t="s">
+      <c r="C64" s="94" t="s">
         <v>129</v>
       </c>
-      <c r="D64" s="110"/>
-      <c r="E64" s="110"/>
+      <c r="D64" s="95"/>
+      <c r="E64" s="95"/>
       <c r="F64" s="96"/>
       <c r="G64" s="30"/>
       <c r="H64" t="s">
@@ -4827,31 +4830,31 @@
       </c>
       <c r="I64" s="30"/>
       <c r="J64" s="28"/>
-      <c r="K64" s="111"/>
-      <c r="L64" s="98"/>
+      <c r="K64" s="103"/>
+      <c r="L64" s="88"/>
     </row>
     <row r="65" spans="1:12" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="30"/>
       <c r="B65" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="C65" s="103"/>
-      <c r="D65" s="104"/>
-      <c r="E65" s="104"/>
-      <c r="F65" s="105"/>
+      <c r="C65" s="104"/>
+      <c r="D65" s="105"/>
+      <c r="E65" s="105"/>
+      <c r="F65" s="106"/>
       <c r="G65" s="30"/>
       <c r="I65" s="30"/>
       <c r="J65" s="28"/>
-      <c r="K65" s="111"/>
-      <c r="L65" s="98"/>
+      <c r="K65" s="103"/>
+      <c r="L65" s="88"/>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A66" s="30"/>
       <c r="G66" s="30"/>
       <c r="I66" s="30"/>
       <c r="J66" s="28"/>
-      <c r="K66" s="111"/>
-      <c r="L66" s="98"/>
+      <c r="K66" s="103"/>
+      <c r="L66" s="88"/>
     </row>
     <row r="67" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="31"/>
@@ -4874,8 +4877,8 @@
       <c r="G68" s="30"/>
       <c r="I68" s="30"/>
       <c r="J68" s="28"/>
-      <c r="K68" s="100"/>
-      <c r="L68" s="98"/>
+      <c r="K68" s="98"/>
+      <c r="L68" s="88"/>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A69" s="50"/>
@@ -4888,8 +4891,8 @@
       <c r="H69" s="52"/>
       <c r="I69" s="50"/>
       <c r="J69" s="53"/>
-      <c r="K69" s="101"/>
-      <c r="L69" s="102"/>
+      <c r="K69" s="107"/>
+      <c r="L69" s="108"/>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A70" s="54"/>
@@ -4910,10 +4913,10 @@
       <c r="E71" s="16"/>
       <c r="F71" s="16"/>
       <c r="G71" s="17"/>
-      <c r="H71" s="107" t="s">
+      <c r="H71" s="92" t="s">
         <v>15</v>
       </c>
-      <c r="I71" s="108"/>
+      <c r="I71" s="93"/>
       <c r="J71" s="14"/>
       <c r="K71" s="18"/>
       <c r="L71" s="14" t="s">
@@ -4943,15 +4946,15 @@
       <c r="B73" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C73" s="103"/>
-      <c r="D73" s="104"/>
-      <c r="E73" s="104"/>
-      <c r="F73" s="105"/>
+      <c r="C73" s="104"/>
+      <c r="D73" s="105"/>
+      <c r="E73" s="105"/>
+      <c r="F73" s="106"/>
       <c r="G73" s="30"/>
       <c r="I73" s="30"/>
       <c r="J73" s="28"/>
-      <c r="K73" s="106"/>
-      <c r="L73" s="109"/>
+      <c r="K73" s="109"/>
+      <c r="L73" s="110"/>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A74" s="30"/>
@@ -4970,8 +4973,8 @@
       </c>
       <c r="I74" s="30"/>
       <c r="J74" s="28"/>
-      <c r="K74" s="97"/>
-      <c r="L74" s="98"/>
+      <c r="K74" s="101"/>
+      <c r="L74" s="88"/>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A75" s="30"/>
@@ -4985,8 +4988,8 @@
       <c r="G75" s="30"/>
       <c r="I75" s="30"/>
       <c r="J75" s="28"/>
-      <c r="K75" s="97"/>
-      <c r="L75" s="98"/>
+      <c r="K75" s="101"/>
+      <c r="L75" s="88"/>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A76" s="30"/>
@@ -5000,16 +5003,16 @@
       <c r="G76" s="30"/>
       <c r="I76" s="30"/>
       <c r="J76" s="28"/>
-      <c r="K76" s="97"/>
-      <c r="L76" s="98"/>
+      <c r="K76" s="101"/>
+      <c r="L76" s="88"/>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A77" s="30"/>
       <c r="G77" s="30"/>
       <c r="I77" s="30"/>
       <c r="J77" s="28"/>
-      <c r="K77" s="97"/>
-      <c r="L77" s="98"/>
+      <c r="K77" s="101"/>
+      <c r="L77" s="88"/>
     </row>
     <row r="78" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="31"/>
@@ -5032,15 +5035,15 @@
       <c r="B79" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C79" s="103"/>
-      <c r="D79" s="104"/>
-      <c r="E79" s="104"/>
-      <c r="F79" s="105"/>
+      <c r="C79" s="104"/>
+      <c r="D79" s="105"/>
+      <c r="E79" s="105"/>
+      <c r="F79" s="106"/>
       <c r="G79" s="30"/>
       <c r="I79" s="30"/>
       <c r="J79" s="28"/>
-      <c r="K79" s="106"/>
-      <c r="L79" s="98"/>
+      <c r="K79" s="109"/>
+      <c r="L79" s="88"/>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A80" s="30"/>
@@ -5059,8 +5062,8 @@
       </c>
       <c r="I80" s="30"/>
       <c r="J80" s="28"/>
-      <c r="K80" s="97"/>
-      <c r="L80" s="98"/>
+      <c r="K80" s="101"/>
+      <c r="L80" s="88"/>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A81" s="30"/>
@@ -5077,8 +5080,8 @@
       <c r="H81" s="61"/>
       <c r="I81" s="30"/>
       <c r="J81" s="28"/>
-      <c r="K81" s="97"/>
-      <c r="L81" s="98"/>
+      <c r="K81" s="101"/>
+      <c r="L81" s="88"/>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A82" s="30"/>
@@ -5093,8 +5096,8 @@
       <c r="H82" s="61"/>
       <c r="I82" s="30"/>
       <c r="J82" s="28"/>
-      <c r="K82" s="97"/>
-      <c r="L82" s="98"/>
+      <c r="K82" s="101"/>
+      <c r="L82" s="88"/>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A83" s="30"/>
@@ -5102,8 +5105,8 @@
       <c r="H83" s="61"/>
       <c r="I83" s="30"/>
       <c r="J83" s="28"/>
-      <c r="K83" s="97"/>
-      <c r="L83" s="98"/>
+      <c r="K83" s="101"/>
+      <c r="L83" s="88"/>
     </row>
     <row r="84" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="31"/>
@@ -5126,15 +5129,15 @@
       <c r="B85" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C85" s="103"/>
-      <c r="D85" s="104"/>
-      <c r="E85" s="104"/>
-      <c r="F85" s="105"/>
+      <c r="C85" s="104"/>
+      <c r="D85" s="105"/>
+      <c r="E85" s="105"/>
+      <c r="F85" s="106"/>
       <c r="G85" s="30"/>
       <c r="I85" s="30"/>
       <c r="J85" s="28"/>
-      <c r="K85" s="106"/>
-      <c r="L85" s="98"/>
+      <c r="K85" s="109"/>
+      <c r="L85" s="88"/>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A86" s="30"/>
@@ -5153,8 +5156,8 @@
       </c>
       <c r="I86" s="30"/>
       <c r="J86" s="30"/>
-      <c r="K86" s="97"/>
-      <c r="L86" s="98"/>
+      <c r="K86" s="101"/>
+      <c r="L86" s="88"/>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A87" s="30"/>
@@ -5169,8 +5172,8 @@
       <c r="H87" s="61"/>
       <c r="I87" s="30"/>
       <c r="J87" s="30"/>
-      <c r="K87" s="97"/>
-      <c r="L87" s="98"/>
+      <c r="K87" s="101"/>
+      <c r="L87" s="88"/>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A88" s="30"/>
@@ -5185,8 +5188,8 @@
       <c r="H88" s="61"/>
       <c r="I88" s="30"/>
       <c r="J88" s="30"/>
-      <c r="K88" s="97"/>
-      <c r="L88" s="98"/>
+      <c r="K88" s="101"/>
+      <c r="L88" s="88"/>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A89" s="30"/>
@@ -5194,8 +5197,8 @@
       <c r="H89" s="61"/>
       <c r="I89" s="30"/>
       <c r="J89" s="30"/>
-      <c r="K89" s="97"/>
-      <c r="L89" s="98"/>
+      <c r="K89" s="101"/>
+      <c r="L89" s="88"/>
     </row>
     <row r="90" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="31"/>
@@ -5218,16 +5221,16 @@
       <c r="G91" s="30"/>
       <c r="I91" s="30"/>
       <c r="J91" s="30"/>
-      <c r="K91" s="100"/>
-      <c r="L91" s="98"/>
+      <c r="K91" s="98"/>
+      <c r="L91" s="88"/>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A92" s="30"/>
       <c r="G92" s="30"/>
       <c r="I92" s="30"/>
       <c r="J92" s="30"/>
-      <c r="K92" s="100"/>
-      <c r="L92" s="98"/>
+      <c r="K92" s="98"/>
+      <c r="L92" s="88"/>
     </row>
     <row r="93" spans="1:12" ht="6" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="31"/>
@@ -5250,16 +5253,16 @@
       <c r="G94" s="30"/>
       <c r="I94" s="30"/>
       <c r="J94" s="30"/>
-      <c r="K94" s="100"/>
-      <c r="L94" s="98"/>
+      <c r="K94" s="98"/>
+      <c r="L94" s="88"/>
     </row>
     <row r="95" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A95" s="30"/>
       <c r="G95" s="30"/>
       <c r="I95" s="30"/>
       <c r="J95" s="30"/>
-      <c r="K95" s="100"/>
-      <c r="L95" s="98"/>
+      <c r="K95" s="98"/>
+      <c r="L95" s="88"/>
     </row>
     <row r="96" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="31"/>
@@ -5286,8 +5289,8 @@
       <c r="G97" s="30"/>
       <c r="I97" s="30"/>
       <c r="J97" s="30"/>
-      <c r="K97" s="97"/>
-      <c r="L97" s="98"/>
+      <c r="K97" s="101"/>
+      <c r="L97" s="88"/>
     </row>
     <row r="98" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A98" s="30"/>
@@ -5303,8 +5306,8 @@
       </c>
       <c r="I98" s="30"/>
       <c r="J98" s="30"/>
-      <c r="K98" s="97"/>
-      <c r="L98" s="98"/>
+      <c r="K98" s="101"/>
+      <c r="L98" s="88"/>
     </row>
     <row r="99" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A99" s="30"/>
@@ -5318,16 +5321,16 @@
       <c r="G99" s="30"/>
       <c r="I99" s="30"/>
       <c r="J99" s="30"/>
-      <c r="K99" s="97"/>
-      <c r="L99" s="98"/>
+      <c r="K99" s="101"/>
+      <c r="L99" s="88"/>
     </row>
     <row r="100" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A100" s="30"/>
       <c r="G100" s="30"/>
       <c r="I100" s="30"/>
       <c r="J100" s="30"/>
-      <c r="K100" s="97"/>
-      <c r="L100" s="98"/>
+      <c r="K100" s="101"/>
+      <c r="L100" s="88"/>
     </row>
     <row r="101" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="31"/>
@@ -5347,7 +5350,7 @@
       <c r="A102" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="B102" s="95" t="s">
+      <c r="B102" s="94" t="s">
         <v>71</v>
       </c>
       <c r="C102" s="96"/>
@@ -5364,8 +5367,8 @@
       </c>
       <c r="I102" s="30"/>
       <c r="J102" s="30"/>
-      <c r="K102" s="97"/>
-      <c r="L102" s="98"/>
+      <c r="K102" s="101"/>
+      <c r="L102" s="88"/>
     </row>
     <row r="103" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A103" s="30"/>
@@ -5373,8 +5376,8 @@
       <c r="G103" s="30"/>
       <c r="I103" s="30"/>
       <c r="J103" s="30"/>
-      <c r="K103" s="97"/>
-      <c r="L103" s="98"/>
+      <c r="K103" s="101"/>
+      <c r="L103" s="88"/>
     </row>
     <row r="104" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="31"/>
@@ -5397,16 +5400,16 @@
       <c r="G105" s="30"/>
       <c r="I105" s="30"/>
       <c r="J105" s="30"/>
-      <c r="K105" s="99"/>
-      <c r="L105" s="98"/>
+      <c r="K105" s="121"/>
+      <c r="L105" s="88"/>
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A106" s="30"/>
       <c r="G106" s="30"/>
       <c r="I106" s="30"/>
       <c r="J106" s="30"/>
-      <c r="K106" s="99"/>
-      <c r="L106" s="98"/>
+      <c r="K106" s="121"/>
+      <c r="L106" s="88"/>
     </row>
     <row r="107" spans="1:12" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="31"/>
@@ -5429,16 +5432,16 @@
       <c r="G108" s="30"/>
       <c r="I108" s="30"/>
       <c r="J108" s="30"/>
-      <c r="K108" s="100"/>
-      <c r="L108" s="98"/>
+      <c r="K108" s="98"/>
+      <c r="L108" s="88"/>
     </row>
     <row r="109" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A109" s="30"/>
       <c r="G109" s="30"/>
       <c r="I109" s="30"/>
       <c r="J109" s="30"/>
-      <c r="K109" s="101"/>
-      <c r="L109" s="102"/>
+      <c r="K109" s="107"/>
+      <c r="L109" s="108"/>
     </row>
     <row r="110" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A110" s="56" t="s">
@@ -5464,10 +5467,10 @@
       <c r="G111" s="30"/>
       <c r="I111" s="30"/>
       <c r="J111" s="30"/>
-      <c r="K111" s="85" t="s">
+      <c r="K111" s="111" t="s">
         <v>127</v>
       </c>
-      <c r="L111" s="86"/>
+      <c r="L111" s="112"/>
     </row>
     <row r="112" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A112" s="30"/>
@@ -5475,8 +5478,8 @@
       <c r="G112" s="30"/>
       <c r="I112" s="30"/>
       <c r="J112" s="30"/>
-      <c r="K112" s="87"/>
-      <c r="L112" s="88"/>
+      <c r="K112" s="113"/>
+      <c r="L112" s="114"/>
     </row>
     <row r="113" spans="1:12" ht="4" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="31"/>
@@ -5499,10 +5502,10 @@
       <c r="G114" s="30"/>
       <c r="I114" s="30"/>
       <c r="J114" s="30"/>
-      <c r="K114" s="85" t="s">
+      <c r="K114" s="111" t="s">
         <v>127</v>
       </c>
-      <c r="L114" s="86"/>
+      <c r="L114" s="112"/>
     </row>
     <row r="115" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A115" s="53"/>
@@ -5515,34 +5518,34 @@
       <c r="H115" s="52"/>
       <c r="I115" s="50"/>
       <c r="J115" s="30"/>
-      <c r="K115" s="89"/>
-      <c r="L115" s="90"/>
+      <c r="K115" s="115"/>
+      <c r="L115" s="116"/>
     </row>
     <row r="116" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J116" s="69" t="s">
         <v>76</v>
       </c>
       <c r="K116" s="70"/>
-      <c r="L116" s="91" t="s">
+      <c r="L116" s="117" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="117" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J117" s="71"/>
       <c r="K117" s="50"/>
-      <c r="L117" s="92"/>
+      <c r="L117" s="118"/>
     </row>
     <row r="118" spans="1:12" x14ac:dyDescent="0.2">
       <c r="J118" s="72" t="s">
         <v>77</v>
       </c>
       <c r="K118" s="27"/>
-      <c r="L118" s="93"/>
+      <c r="L118" s="119"/>
     </row>
     <row r="119" spans="1:12" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="J119" s="73"/>
       <c r="K119" s="74"/>
-      <c r="L119" s="94"/>
+      <c r="L119" s="120"/>
     </row>
     <row r="121" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A121" s="56" t="s">
@@ -5795,30 +5798,36 @@
     </row>
   </sheetData>
   <mergeCells count="70">
-    <mergeCell ref="L18:L19"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="K21:K22"/>
-    <mergeCell ref="L21:L22"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="K24:K27"/>
-    <mergeCell ref="L24:L27"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="K29:K31"/>
-    <mergeCell ref="L29:L31"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="K33:K35"/>
-    <mergeCell ref="L33:L35"/>
-    <mergeCell ref="K37:K38"/>
-    <mergeCell ref="L37:L38"/>
-    <mergeCell ref="C40:F40"/>
-    <mergeCell ref="K40:K44"/>
-    <mergeCell ref="L40:L44"/>
-    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="K111:L112"/>
+    <mergeCell ref="K114:L115"/>
+    <mergeCell ref="L116:L117"/>
+    <mergeCell ref="L118:L119"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="K102:K103"/>
+    <mergeCell ref="L102:L103"/>
+    <mergeCell ref="K105:K106"/>
+    <mergeCell ref="L105:L106"/>
+    <mergeCell ref="K108:K109"/>
+    <mergeCell ref="L108:L109"/>
+    <mergeCell ref="K91:K92"/>
+    <mergeCell ref="L91:L92"/>
+    <mergeCell ref="K94:K95"/>
+    <mergeCell ref="L94:L95"/>
+    <mergeCell ref="K97:K100"/>
+    <mergeCell ref="L97:L100"/>
+    <mergeCell ref="C79:F79"/>
+    <mergeCell ref="K79:K83"/>
+    <mergeCell ref="L79:L83"/>
+    <mergeCell ref="C85:F85"/>
+    <mergeCell ref="K85:K89"/>
+    <mergeCell ref="L85:L89"/>
+    <mergeCell ref="C60:F60"/>
+    <mergeCell ref="K68:K69"/>
+    <mergeCell ref="L68:L69"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="K73:K77"/>
+    <mergeCell ref="L73:L77"/>
     <mergeCell ref="C64:F64"/>
     <mergeCell ref="K64:K66"/>
     <mergeCell ref="L64:L66"/>
@@ -5835,36 +5844,30 @@
     <mergeCell ref="K58:K62"/>
     <mergeCell ref="L58:L62"/>
     <mergeCell ref="C59:F59"/>
-    <mergeCell ref="C60:F60"/>
-    <mergeCell ref="K68:K69"/>
-    <mergeCell ref="L68:L69"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="K73:K77"/>
-    <mergeCell ref="L73:L77"/>
-    <mergeCell ref="C79:F79"/>
-    <mergeCell ref="K79:K83"/>
-    <mergeCell ref="L79:L83"/>
-    <mergeCell ref="C85:F85"/>
-    <mergeCell ref="K85:K89"/>
-    <mergeCell ref="L85:L89"/>
-    <mergeCell ref="K91:K92"/>
-    <mergeCell ref="L91:L92"/>
-    <mergeCell ref="K94:K95"/>
-    <mergeCell ref="L94:L95"/>
-    <mergeCell ref="K97:K100"/>
-    <mergeCell ref="L97:L100"/>
-    <mergeCell ref="K111:L112"/>
-    <mergeCell ref="K114:L115"/>
-    <mergeCell ref="L116:L117"/>
-    <mergeCell ref="L118:L119"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="K102:K103"/>
-    <mergeCell ref="L102:L103"/>
-    <mergeCell ref="K105:K106"/>
-    <mergeCell ref="L105:L106"/>
-    <mergeCell ref="K108:K109"/>
-    <mergeCell ref="L108:L109"/>
+    <mergeCell ref="K37:K38"/>
+    <mergeCell ref="L37:L38"/>
+    <mergeCell ref="C40:F40"/>
+    <mergeCell ref="K40:K44"/>
+    <mergeCell ref="L40:L44"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="K29:K31"/>
+    <mergeCell ref="L29:L31"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="K33:K35"/>
+    <mergeCell ref="L33:L35"/>
+    <mergeCell ref="K21:K22"/>
+    <mergeCell ref="L21:L22"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="K24:K27"/>
+    <mergeCell ref="L24:L27"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="C26:E26"/>
+    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="K18:K19"/>
   </mergeCells>
   <conditionalFormatting sqref="B97">
     <cfRule type="expression" dxfId="327" priority="10">

</xml_diff>